<commit_message>
read excel file with specific sheet name `input_data`
</commit_message>
<xml_diff>
--- a/masterinput.xlsx
+++ b/masterinput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\PycharmProjects\auto-input-BMKGSatu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8552BCD9-25AF-442B-8DD1-9700A92108D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392AC6EF-9A3A-4C42-ADBA-FD4C62346EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68302FD9-38CD-42FA-91E9-66E8EDD65E83}"/>
   </bookViews>
@@ -542,7 +542,7 @@
   <dimension ref="A1:AQ25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>